<commit_message>
some small manual SS calibration to get model in ball park
</commit_message>
<xml_diff>
--- a/Simulation_20161129_SteadyState/Excel_info/Streamflow_1992_2003_Aves.xlsx
+++ b/Simulation_20161129_SteadyState/Excel_info/Streamflow_1992_2003_Aves.xlsx
@@ -373,7 +373,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -405,6 +405,14 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="90"/>
     </xf>
@@ -426,14 +434,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -779,10 +780,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:P38"/>
+  <dimension ref="A2:Q38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -792,25 +793,25 @@
     <col min="3" max="10" width="10.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B2" s="38" t="s">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B2" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
-      <c r="K2" s="39"/>
-      <c r="L2" s="39"/>
-      <c r="M2" s="39"/>
-      <c r="N2" s="39"/>
-      <c r="O2" s="40"/>
-    </row>
-    <row r="3" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="33"/>
+      <c r="J2" s="33"/>
+      <c r="K2" s="33"/>
+      <c r="L2" s="33"/>
+      <c r="M2" s="33"/>
+      <c r="N2" s="33"/>
+      <c r="O2" s="34"/>
+    </row>
+    <row r="3" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B3" s="13" t="s">
         <v>26</v>
       </c>
@@ -857,8 +858,8 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A4" s="36" t="s">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A4" s="40" t="s">
         <v>28</v>
       </c>
       <c r="B4" s="9" t="s">
@@ -904,13 +905,13 @@
         <f>AVERAGE(C4:N4)</f>
         <v>8.1990474166666694</v>
       </c>
-      <c r="P4" s="41">
+      <c r="P4" s="31">
         <f>86400*O4*0.3048^3</f>
         <v>20059.58890641174</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A5" s="37"/>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A5" s="41"/>
       <c r="B5" s="9" t="s">
         <v>1</v>
       </c>
@@ -954,13 +955,13 @@
         <f t="shared" ref="O5:O18" si="0">AVERAGE(C5:N5)</f>
         <v>16.264622916666664</v>
       </c>
-      <c r="P5" s="41">
+      <c r="P5" s="31">
         <f t="shared" ref="P5:P18" si="1">86400*O5*0.3048^3</f>
         <v>39792.628685489261</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A6" s="37"/>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A6" s="41"/>
       <c r="B6" s="9" t="s">
         <v>2</v>
       </c>
@@ -1004,13 +1005,13 @@
         <f t="shared" si="0"/>
         <v>130.32311508333336</v>
       </c>
-      <c r="P6" s="41">
+      <c r="P6" s="31">
         <f t="shared" si="1"/>
         <v>318845.3463826254</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A7" s="37"/>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A7" s="41"/>
       <c r="B7" s="9" t="s">
         <v>3</v>
       </c>
@@ -1054,13 +1055,13 @@
         <f t="shared" si="0"/>
         <v>10.132239671666667</v>
       </c>
-      <c r="P7" s="41">
+      <c r="P7" s="31">
         <f t="shared" si="1"/>
         <v>24789.289802339074</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A8" s="37"/>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A8" s="41"/>
       <c r="B8" s="9" t="s">
         <v>4</v>
       </c>
@@ -1104,13 +1105,13 @@
         <f t="shared" si="0"/>
         <v>3.3061217941666672</v>
       </c>
-      <c r="P8" s="41">
+      <c r="P8" s="31">
         <f t="shared" si="1"/>
         <v>8088.6767322140931</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A9" s="37"/>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A9" s="41"/>
       <c r="B9" s="9" t="s">
         <v>5</v>
       </c>
@@ -1154,13 +1155,14 @@
         <f t="shared" si="0"/>
         <v>131.94677422499998</v>
       </c>
-      <c r="P9" s="41">
+      <c r="P9" s="31">
         <f>86400*O9*0.3048^3</f>
         <v>322817.75113293371</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A10" s="37"/>
+      <c r="Q9" s="42"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A10" s="41"/>
       <c r="B10" s="9" t="s">
         <v>6</v>
       </c>
@@ -1204,13 +1206,13 @@
         <f t="shared" si="0"/>
         <v>1.0107492916666667</v>
       </c>
-      <c r="P10" s="41">
+      <c r="P10" s="31">
         <f t="shared" si="1"/>
         <v>2472.8744996724386</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A11" s="37"/>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A11" s="41"/>
       <c r="B11" s="9" t="s">
         <v>7</v>
       </c>
@@ -1254,13 +1256,13 @@
         <f t="shared" si="0"/>
         <v>9.1800711666666661</v>
       </c>
-      <c r="P11" s="41">
+      <c r="P11" s="31">
         <f t="shared" si="1"/>
         <v>22459.737622764311</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A12" s="37"/>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A12" s="41"/>
       <c r="B12" s="9" t="s">
         <v>8</v>
       </c>
@@ -1304,13 +1306,13 @@
         <f t="shared" si="0"/>
         <v>1.6937752916666666</v>
       </c>
-      <c r="P12" s="41">
+      <c r="P12" s="31">
         <f t="shared" si="1"/>
         <v>4143.949208246454</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A13" s="37"/>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A13" s="41"/>
       <c r="B13" s="9" t="s">
         <v>9</v>
       </c>
@@ -1354,13 +1356,13 @@
         <f t="shared" si="0"/>
         <v>2.0611517141666669</v>
       </c>
-      <c r="P13" s="41">
+      <c r="P13" s="31">
         <f t="shared" si="1"/>
         <v>5042.7633795461579</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A14" s="37"/>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A14" s="41"/>
       <c r="B14" s="9" t="s">
         <v>10</v>
       </c>
@@ -1404,13 +1406,13 @@
         <f t="shared" si="0"/>
         <v>62.272262333333352</v>
       </c>
-      <c r="P14" s="41">
+      <c r="P14" s="31">
         <f t="shared" si="1"/>
         <v>152353.79419073305</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A15" s="37"/>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A15" s="41"/>
       <c r="B15" s="9" t="s">
         <v>11</v>
       </c>
@@ -1454,13 +1456,13 @@
         <f t="shared" si="0"/>
         <v>5.7139664166666675</v>
       </c>
-      <c r="P15" s="41">
+      <c r="P15" s="31">
         <f t="shared" si="1"/>
         <v>13979.650503103776</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A16" s="37"/>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A16" s="41"/>
       <c r="B16" s="9" t="s">
         <v>27</v>
       </c>
@@ -1504,13 +1506,13 @@
         <f t="shared" si="0"/>
         <v>45.159474166666676</v>
       </c>
-      <c r="P16" s="41">
+      <c r="P16" s="31">
         <f t="shared" si="1"/>
         <v>110486.06514600948</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A17" s="31" t="s">
+      <c r="A17" s="35" t="s">
         <v>29</v>
       </c>
       <c r="B17" s="27" t="s">
@@ -1556,13 +1558,13 @@
         <f t="shared" si="0"/>
         <v>128.85825333333332</v>
       </c>
-      <c r="P17" s="41">
+      <c r="P17" s="31">
         <f t="shared" si="1"/>
         <v>315261.45144746552</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A18" s="32"/>
+      <c r="A18" s="36"/>
       <c r="B18" s="10" t="s">
         <v>13</v>
       </c>
@@ -1606,7 +1608,7 @@
         <f t="shared" si="0"/>
         <v>123.71298208333333</v>
       </c>
-      <c r="P18" s="41">
+      <c r="P18" s="31">
         <f t="shared" si="1"/>
         <v>302673.15663200017</v>
       </c>
@@ -1665,21 +1667,21 @@
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B22" s="33" t="s">
+      <c r="B22" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="C22" s="34"/>
-      <c r="D22" s="34"/>
-      <c r="E22" s="34"/>
-      <c r="F22" s="34"/>
-      <c r="G22" s="34"/>
-      <c r="H22" s="34"/>
-      <c r="I22" s="34"/>
-      <c r="J22" s="34"/>
-      <c r="K22" s="34"/>
-      <c r="L22" s="34"/>
-      <c r="M22" s="34"/>
-      <c r="N22" s="35"/>
+      <c r="C22" s="38"/>
+      <c r="D22" s="38"/>
+      <c r="E22" s="38"/>
+      <c r="F22" s="38"/>
+      <c r="G22" s="38"/>
+      <c r="H22" s="38"/>
+      <c r="I22" s="38"/>
+      <c r="J22" s="38"/>
+      <c r="K22" s="38"/>
+      <c r="L22" s="38"/>
+      <c r="M22" s="38"/>
+      <c r="N22" s="39"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B23" s="17" t="s">
@@ -1723,7 +1725,7 @@
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A24" s="36" t="s">
+      <c r="A24" s="40" t="s">
         <v>28</v>
       </c>
       <c r="B24" s="21" t="s">
@@ -1751,7 +1753,7 @@
       <c r="N24" s="25"/>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A25" s="37"/>
+      <c r="A25" s="41"/>
       <c r="B25" s="21" t="s">
         <v>1</v>
       </c>
@@ -1777,7 +1779,7 @@
       <c r="N25" s="3"/>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A26" s="37"/>
+      <c r="A26" s="41"/>
       <c r="B26" s="21" t="s">
         <v>2</v>
       </c>
@@ -1803,7 +1805,7 @@
       <c r="N26" s="3"/>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A27" s="37"/>
+      <c r="A27" s="41"/>
       <c r="B27" s="21" t="s">
         <v>3</v>
       </c>
@@ -1829,7 +1831,7 @@
       <c r="N27" s="3"/>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A28" s="37"/>
+      <c r="A28" s="41"/>
       <c r="B28" s="21" t="s">
         <v>4</v>
       </c>
@@ -1855,7 +1857,7 @@
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A29" s="37"/>
+      <c r="A29" s="41"/>
       <c r="B29" s="21" t="s">
         <v>5</v>
       </c>
@@ -1881,7 +1883,7 @@
       <c r="N29" s="3"/>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A30" s="37"/>
+      <c r="A30" s="41"/>
       <c r="B30" s="21" t="s">
         <v>6</v>
       </c>
@@ -1907,7 +1909,7 @@
       <c r="N30" s="3"/>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A31" s="37"/>
+      <c r="A31" s="41"/>
       <c r="B31" s="21" t="s">
         <v>7</v>
       </c>
@@ -1933,7 +1935,7 @@
       <c r="N31" s="3"/>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A32" s="37"/>
+      <c r="A32" s="41"/>
       <c r="B32" s="21" t="s">
         <v>8</v>
       </c>
@@ -1959,7 +1961,7 @@
       <c r="N32" s="3"/>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A33" s="37"/>
+      <c r="A33" s="41"/>
       <c r="B33" s="21" t="s">
         <v>9</v>
       </c>
@@ -1985,7 +1987,7 @@
       <c r="N33" s="3"/>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A34" s="37"/>
+      <c r="A34" s="41"/>
       <c r="B34" s="21" t="s">
         <v>10</v>
       </c>
@@ -2011,7 +2013,7 @@
       <c r="N34" s="3"/>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A35" s="37"/>
+      <c r="A35" s="41"/>
       <c r="B35" s="21" t="s">
         <v>11</v>
       </c>
@@ -2037,7 +2039,7 @@
       <c r="N35" s="3"/>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A36" s="37"/>
+      <c r="A36" s="41"/>
       <c r="B36" s="21" t="s">
         <v>27</v>
       </c>
@@ -2063,7 +2065,7 @@
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A37" s="31" t="s">
+      <c r="A37" s="35" t="s">
         <v>29</v>
       </c>
       <c r="B37" s="26" t="s">
@@ -2091,7 +2093,7 @@
       <c r="N37" s="25"/>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A38" s="32"/>
+      <c r="A38" s="36"/>
       <c r="B38" s="22" t="s">
         <v>13</v>
       </c>

</xml_diff>

<commit_message>
add GWET calcs to worksheet for SS calibration
</commit_message>
<xml_diff>
--- a/Simulation_20161129_SteadyState/Excel_info/Streamflow_1992_2003_Aves.xlsx
+++ b/Simulation_20161129_SteadyState/Excel_info/Streamflow_1992_2003_Aves.xlsx
@@ -5,14 +5,15 @@
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DATA\Niswonger\carmel.git\Simulation_20161129_SteadyState\Excel_info\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DATA\Niswonger\Carmel.git\Simulation_20161129_SteadyState\Excel_info\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="16656" yWindow="1824" windowWidth="28320" windowHeight="19176" tabRatio="500"/>
+    <workbookView xWindow="16656" yWindow="1824" windowWidth="28320" windowHeight="19176" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Streamflow_Averages_1992_2003" sheetId="1" r:id="rId1"/>
+    <sheet name="baseflow GWET calcs" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="48">
   <si>
     <t>CA</t>
   </si>
@@ -129,6 +130,45 @@
   </si>
   <si>
     <t>Ave (CMD)</t>
+  </si>
+  <si>
+    <t>Average runoff at H1 gage</t>
+  </si>
+  <si>
+    <t>Average base flow at H1 gage</t>
+  </si>
+  <si>
+    <t>Fraction  summer covden</t>
+  </si>
+  <si>
+    <t>number of cells with riparian</t>
+  </si>
+  <si>
+    <t>Cell area</t>
+  </si>
+  <si>
+    <t>Area of riparan zone (m2)</t>
+  </si>
+  <si>
+    <t>recharge</t>
+  </si>
+  <si>
+    <t>GW ET</t>
+  </si>
+  <si>
+    <t>Total precip m3/day</t>
+  </si>
+  <si>
+    <t>RCH/PPT</t>
+  </si>
+  <si>
+    <t>GWET (TCH-Qbf)</t>
+  </si>
+  <si>
+    <t>GWET depth m/d</t>
+  </si>
+  <si>
+    <t>GWET depth m/yr</t>
   </si>
 </sst>
 </file>
@@ -406,6 +446,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -434,7 +475,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -780,10 +820,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:Q38"/>
+  <dimension ref="A2:R38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="Q9" sqref="Q9"/>
+    <sheetView topLeftCell="D1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -793,25 +833,25 @@
     <col min="3" max="10" width="10.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B2" s="32" t="s">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B2" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
-      <c r="M2" s="33"/>
-      <c r="N2" s="33"/>
-      <c r="O2" s="34"/>
-    </row>
-    <row r="3" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="34"/>
+      <c r="K2" s="34"/>
+      <c r="L2" s="34"/>
+      <c r="M2" s="34"/>
+      <c r="N2" s="34"/>
+      <c r="O2" s="35"/>
+    </row>
+    <row r="3" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B3" s="13" t="s">
         <v>26</v>
       </c>
@@ -858,8 +898,8 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A4" s="40" t="s">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A4" s="41" t="s">
         <v>28</v>
       </c>
       <c r="B4" s="9" t="s">
@@ -910,8 +950,8 @@
         <v>20059.58890641174</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A5" s="41"/>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A5" s="42"/>
       <c r="B5" s="9" t="s">
         <v>1</v>
       </c>
@@ -960,8 +1000,8 @@
         <v>39792.628685489261</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A6" s="41"/>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A6" s="42"/>
       <c r="B6" s="9" t="s">
         <v>2</v>
       </c>
@@ -1010,8 +1050,8 @@
         <v>318845.3463826254</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A7" s="41"/>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A7" s="42"/>
       <c r="B7" s="9" t="s">
         <v>3</v>
       </c>
@@ -1060,8 +1100,8 @@
         <v>24789.289802339074</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A8" s="41"/>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A8" s="42"/>
       <c r="B8" s="9" t="s">
         <v>4</v>
       </c>
@@ -1110,8 +1150,8 @@
         <v>8088.6767322140931</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A9" s="41"/>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A9" s="42"/>
       <c r="B9" s="9" t="s">
         <v>5</v>
       </c>
@@ -1159,10 +1199,11 @@
         <f>86400*O9*0.3048^3</f>
         <v>322817.75113293371</v>
       </c>
-      <c r="Q9" s="42"/>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A10" s="41"/>
+      <c r="Q9" s="32"/>
+      <c r="R9" s="31"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A10" s="42"/>
       <c r="B10" s="9" t="s">
         <v>6</v>
       </c>
@@ -1211,8 +1252,8 @@
         <v>2472.8744996724386</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A11" s="41"/>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A11" s="42"/>
       <c r="B11" s="9" t="s">
         <v>7</v>
       </c>
@@ -1261,8 +1302,8 @@
         <v>22459.737622764311</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A12" s="41"/>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A12" s="42"/>
       <c r="B12" s="9" t="s">
         <v>8</v>
       </c>
@@ -1311,8 +1352,8 @@
         <v>4143.949208246454</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A13" s="41"/>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A13" s="42"/>
       <c r="B13" s="9" t="s">
         <v>9</v>
       </c>
@@ -1361,8 +1402,8 @@
         <v>5042.7633795461579</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A14" s="41"/>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A14" s="42"/>
       <c r="B14" s="9" t="s">
         <v>10</v>
       </c>
@@ -1411,8 +1452,8 @@
         <v>152353.79419073305</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A15" s="41"/>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A15" s="42"/>
       <c r="B15" s="9" t="s">
         <v>11</v>
       </c>
@@ -1461,8 +1502,8 @@
         <v>13979.650503103776</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A16" s="41"/>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A16" s="42"/>
       <c r="B16" s="9" t="s">
         <v>27</v>
       </c>
@@ -1512,7 +1553,7 @@
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A17" s="35" t="s">
+      <c r="A17" s="36" t="s">
         <v>29</v>
       </c>
       <c r="B17" s="27" t="s">
@@ -1564,7 +1605,7 @@
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A18" s="36"/>
+      <c r="A18" s="37"/>
       <c r="B18" s="10" t="s">
         <v>13</v>
       </c>
@@ -1667,21 +1708,21 @@
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B22" s="37" t="s">
+      <c r="B22" s="38" t="s">
         <v>32</v>
       </c>
-      <c r="C22" s="38"/>
-      <c r="D22" s="38"/>
-      <c r="E22" s="38"/>
-      <c r="F22" s="38"/>
-      <c r="G22" s="38"/>
-      <c r="H22" s="38"/>
-      <c r="I22" s="38"/>
-      <c r="J22" s="38"/>
-      <c r="K22" s="38"/>
-      <c r="L22" s="38"/>
-      <c r="M22" s="38"/>
-      <c r="N22" s="39"/>
+      <c r="C22" s="39"/>
+      <c r="D22" s="39"/>
+      <c r="E22" s="39"/>
+      <c r="F22" s="39"/>
+      <c r="G22" s="39"/>
+      <c r="H22" s="39"/>
+      <c r="I22" s="39"/>
+      <c r="J22" s="39"/>
+      <c r="K22" s="39"/>
+      <c r="L22" s="39"/>
+      <c r="M22" s="39"/>
+      <c r="N22" s="40"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B23" s="17" t="s">
@@ -1725,7 +1766,7 @@
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A24" s="40" t="s">
+      <c r="A24" s="41" t="s">
         <v>28</v>
       </c>
       <c r="B24" s="21" t="s">
@@ -1753,7 +1794,7 @@
       <c r="N24" s="25"/>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A25" s="41"/>
+      <c r="A25" s="42"/>
       <c r="B25" s="21" t="s">
         <v>1</v>
       </c>
@@ -1779,7 +1820,7 @@
       <c r="N25" s="3"/>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A26" s="41"/>
+      <c r="A26" s="42"/>
       <c r="B26" s="21" t="s">
         <v>2</v>
       </c>
@@ -1805,7 +1846,7 @@
       <c r="N26" s="3"/>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A27" s="41"/>
+      <c r="A27" s="42"/>
       <c r="B27" s="21" t="s">
         <v>3</v>
       </c>
@@ -1831,7 +1872,7 @@
       <c r="N27" s="3"/>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A28" s="41"/>
+      <c r="A28" s="42"/>
       <c r="B28" s="21" t="s">
         <v>4</v>
       </c>
@@ -1857,7 +1898,7 @@
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A29" s="41"/>
+      <c r="A29" s="42"/>
       <c r="B29" s="21" t="s">
         <v>5</v>
       </c>
@@ -1883,7 +1924,7 @@
       <c r="N29" s="3"/>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A30" s="41"/>
+      <c r="A30" s="42"/>
       <c r="B30" s="21" t="s">
         <v>6</v>
       </c>
@@ -1909,7 +1950,7 @@
       <c r="N30" s="3"/>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A31" s="41"/>
+      <c r="A31" s="42"/>
       <c r="B31" s="21" t="s">
         <v>7</v>
       </c>
@@ -1935,7 +1976,7 @@
       <c r="N31" s="3"/>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A32" s="41"/>
+      <c r="A32" s="42"/>
       <c r="B32" s="21" t="s">
         <v>8</v>
       </c>
@@ -1961,7 +2002,7 @@
       <c r="N32" s="3"/>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A33" s="41"/>
+      <c r="A33" s="42"/>
       <c r="B33" s="21" t="s">
         <v>9</v>
       </c>
@@ -1987,7 +2028,7 @@
       <c r="N33" s="3"/>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A34" s="41"/>
+      <c r="A34" s="42"/>
       <c r="B34" s="21" t="s">
         <v>10</v>
       </c>
@@ -2013,7 +2054,7 @@
       <c r="N34" s="3"/>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A35" s="41"/>
+      <c r="A35" s="42"/>
       <c r="B35" s="21" t="s">
         <v>11</v>
       </c>
@@ -2039,7 +2080,7 @@
       <c r="N35" s="3"/>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A36" s="41"/>
+      <c r="A36" s="42"/>
       <c r="B36" s="21" t="s">
         <v>27</v>
       </c>
@@ -2065,7 +2106,7 @@
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A37" s="35" t="s">
+      <c r="A37" s="36" t="s">
         <v>29</v>
       </c>
       <c r="B37" s="26" t="s">
@@ -2093,7 +2134,7 @@
       <c r="N37" s="25"/>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A38" s="36"/>
+      <c r="A38" s="37"/>
       <c r="B38" s="22" t="s">
         <v>13</v>
       </c>
@@ -2135,4 +2176,125 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:N5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="23.796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.69921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.09765625" customWidth="1"/>
+    <col min="7" max="7" width="22.69921875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.296875" customWidth="1"/>
+    <col min="9" max="9" width="18" customWidth="1"/>
+    <col min="10" max="11" width="10.3984375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.8984375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.59765625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.09765625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M1" t="s">
+        <v>46</v>
+      </c>
+      <c r="N1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B2">
+        <v>322817.75113293371</v>
+      </c>
+      <c r="C2" s="32">
+        <v>24074.303368200195</v>
+      </c>
+      <c r="D2">
+        <v>0.35299999999999998</v>
+      </c>
+      <c r="E2">
+        <v>11100</v>
+      </c>
+      <c r="F2">
+        <f>100*100</f>
+        <v>10000</v>
+      </c>
+      <c r="G2">
+        <f>D2*E2*F2</f>
+        <v>39183000</v>
+      </c>
+      <c r="H2">
+        <f>G2*0.85/365</f>
+        <v>91248.082191780821</v>
+      </c>
+      <c r="I2">
+        <v>1279516.6399999999</v>
+      </c>
+      <c r="J2" s="31">
+        <v>104541.09239999999</v>
+      </c>
+      <c r="K2" s="31">
+        <f>J2/I2</f>
+        <v>8.1703581752559318E-2</v>
+      </c>
+      <c r="L2" s="31">
+        <f>J2-C2</f>
+        <v>80466.789031799795</v>
+      </c>
+      <c r="M2" s="31">
+        <f>L2/G2</f>
+        <v>2.0536148082535739E-3</v>
+      </c>
+      <c r="N2" s="31">
+        <f>M2*365</f>
+        <v>0.74956940501255453</v>
+      </c>
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="J5" s="32"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added transient stream stremflow file to transiet model directory
</commit_message>
<xml_diff>
--- a/Simulation_20161129_SteadyState/Excel_info/Streamflow_1992_2003_Aves.xlsx
+++ b/Simulation_20161129_SteadyState/Excel_info/Streamflow_1992_2003_Aves.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="16656" yWindow="1824" windowWidth="28320" windowHeight="19176" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="16656" yWindow="1824" windowWidth="28320" windowHeight="19176" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Streamflow_Averages_1992_2003" sheetId="1" r:id="rId1"/>
@@ -822,8 +822,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:R38"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="P9" sqref="P9"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2182,8 +2182,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:N5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2291,6 +2291,12 @@
         <v>0.74956940501255453</v>
       </c>
     </row>
+    <row r="3" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="N3" s="31">
+        <f>N2/0.3048</f>
+        <v>2.4592172080464385</v>
+      </c>
+    </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.3">
       <c r="J5" s="32"/>
     </row>

</xml_diff>